<commit_message>
Email gefixed voor edit & Begeleider gefixedf
</commit_message>
<xml_diff>
--- a/PVB Stage Applicatie/App_Data/uploads/DocentInvoegen.xlsx
+++ b/PVB Stage Applicatie/App_Data/uploads/DocentInvoegen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Voornaam</t>
   </si>
@@ -50,30 +50,6 @@
   </si>
   <si>
     <t>Wachtwoord</t>
-  </si>
-  <si>
-    <t>Bulk</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>werktwel@hotmail.com</t>
-  </si>
-  <si>
-    <t>toch</t>
-  </si>
-  <si>
-    <t>7457ER</t>
-  </si>
-  <si>
-    <t>Enschede</t>
-  </si>
-  <si>
-    <t>BUT</t>
-  </si>
-  <si>
-    <t>but</t>
   </si>
 </sst>
 </file>
@@ -466,7 +442,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,38 +499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="V21ieBGYvRQupL9plkBDTgAV3ZM4NERsWEcuN8YhtHvFqJJG6kmZu5tcGbM2xS10IGLrTB7sx89KCuYrut0Ecw==" saltValue="4SxHEUi9VJ9RUe96YJMwnw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
sp aangepast voor bedrijven bulk koppeling fix
</commit_message>
<xml_diff>
--- a/PVB Stage Applicatie/App_Data/uploads/DocentInvoegen.xlsx
+++ b/PVB Stage Applicatie/App_Data/uploads/DocentInvoegen.xlsx
@@ -61,238 +61,238 @@
     <t>Pieter</t>
   </si>
   <si>
+    <t>Aad</t>
+  </si>
+  <si>
+    <t>Angela</t>
+  </si>
+  <si>
+    <t>Merel</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t>Vincent</t>
+  </si>
+  <si>
+    <t>Wargers</t>
+  </si>
+  <si>
+    <t>Roesink</t>
+  </si>
+  <si>
+    <t>Moens</t>
+  </si>
+  <si>
+    <t>Homans</t>
+  </si>
+  <si>
+    <t>Kaaden</t>
+  </si>
+  <si>
+    <t>Rogge</t>
+  </si>
+  <si>
+    <t>Vink</t>
+  </si>
+  <si>
+    <t>Hee</t>
+  </si>
+  <si>
+    <t>Kroos</t>
+  </si>
+  <si>
+    <t>van der</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>Gwargers@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Mroesink@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Pmoens@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Chomans@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Akaaden@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Arogge@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Mvink@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Ahee@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Vkroos@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Karel</t>
+  </si>
+  <si>
+    <t>Bouter</t>
+  </si>
+  <si>
+    <t>Kbouter@rocvantwente.nl</t>
+  </si>
+  <si>
+    <t>Enschedesestraat</t>
+  </si>
+  <si>
+    <t>Enktermorsweg</t>
+  </si>
+  <si>
+    <t>Hoge Linde</t>
+  </si>
+  <si>
+    <t>Lage Linde</t>
+  </si>
+  <si>
+    <t>Middelgrote Linde</t>
+  </si>
+  <si>
+    <t>Huisweg</t>
+  </si>
+  <si>
+    <t>Tornadolaan</t>
+  </si>
+  <si>
+    <t>De Mors</t>
+  </si>
+  <si>
+    <t>Kalaan</t>
+  </si>
+  <si>
+    <t>Slotsweg</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>1348RY</t>
+  </si>
+  <si>
+    <t>9238OO</t>
+  </si>
+  <si>
+    <t>3848UU</t>
+  </si>
+  <si>
+    <t>6469BN</t>
+  </si>
+  <si>
+    <t>2309JG</t>
+  </si>
+  <si>
+    <t>6842UP</t>
+  </si>
+  <si>
+    <t>8701ER</t>
+  </si>
+  <si>
+    <t>2948II</t>
+  </si>
+  <si>
+    <t>2030PP</t>
+  </si>
+  <si>
+    <t>8239TT</t>
+  </si>
+  <si>
+    <t>Enschede</t>
+  </si>
+  <si>
+    <t>Denekamp</t>
+  </si>
+  <si>
+    <t>Ootmarsum</t>
+  </si>
+  <si>
+    <t>Oldenzaal</t>
+  </si>
+  <si>
+    <t>Neede</t>
+  </si>
+  <si>
+    <t>Losser</t>
+  </si>
+  <si>
+    <t>Hengelo</t>
+  </si>
+  <si>
+    <t>Almelo</t>
+  </si>
+  <si>
+    <t>WAG</t>
+  </si>
+  <si>
+    <t>RSK</t>
+  </si>
+  <si>
+    <t>MNS</t>
+  </si>
+  <si>
+    <t>HMN</t>
+  </si>
+  <si>
+    <t>KAD</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>ROG</t>
+  </si>
+  <si>
+    <t>VIK</t>
+  </si>
+  <si>
+    <t>HEE</t>
+  </si>
+  <si>
+    <t>KRO</t>
+  </si>
+  <si>
+    <t>gerard</t>
+  </si>
+  <si>
+    <t>marcel</t>
+  </si>
+  <si>
+    <t>pieter</t>
+  </si>
+  <si>
+    <t>cees</t>
+  </si>
+  <si>
+    <t>aad</t>
+  </si>
+  <si>
+    <t>karel</t>
+  </si>
+  <si>
+    <t>angela</t>
+  </si>
+  <si>
+    <t>merel</t>
+  </si>
+  <si>
+    <t>arnold</t>
+  </si>
+  <si>
+    <t>vincent</t>
+  </si>
+  <si>
     <t>Cees</t>
-  </si>
-  <si>
-    <t>Aad</t>
-  </si>
-  <si>
-    <t>Angela</t>
-  </si>
-  <si>
-    <t>Merel</t>
-  </si>
-  <si>
-    <t>Arnold</t>
-  </si>
-  <si>
-    <t>Vincent</t>
-  </si>
-  <si>
-    <t>Wargers</t>
-  </si>
-  <si>
-    <t>Roesink</t>
-  </si>
-  <si>
-    <t>Moens</t>
-  </si>
-  <si>
-    <t>Homans</t>
-  </si>
-  <si>
-    <t>Kaaden</t>
-  </si>
-  <si>
-    <t>Rogge</t>
-  </si>
-  <si>
-    <t>Vink</t>
-  </si>
-  <si>
-    <t>Hee</t>
-  </si>
-  <si>
-    <t>Kroos</t>
-  </si>
-  <si>
-    <t>van der</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>Gwargers@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Mroesink@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Pmoens@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Chomans@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Akaaden@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Arogge@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Mvink@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Ahee@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Vkroos@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Karel</t>
-  </si>
-  <si>
-    <t>Bouter</t>
-  </si>
-  <si>
-    <t>Kbouter@rocvantwente.nl</t>
-  </si>
-  <si>
-    <t>Enschedesestraat</t>
-  </si>
-  <si>
-    <t>Enktermorsweg</t>
-  </si>
-  <si>
-    <t>Hoge Linde</t>
-  </si>
-  <si>
-    <t>Lage Linde</t>
-  </si>
-  <si>
-    <t>Middelgrote Linde</t>
-  </si>
-  <si>
-    <t>Huisweg</t>
-  </si>
-  <si>
-    <t>Tornadolaan</t>
-  </si>
-  <si>
-    <t>De Mors</t>
-  </si>
-  <si>
-    <t>Kalaan</t>
-  </si>
-  <si>
-    <t>Slotsweg</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>1348RY</t>
-  </si>
-  <si>
-    <t>9238OO</t>
-  </si>
-  <si>
-    <t>3848UU</t>
-  </si>
-  <si>
-    <t>6469BN</t>
-  </si>
-  <si>
-    <t>2309JG</t>
-  </si>
-  <si>
-    <t>6842UP</t>
-  </si>
-  <si>
-    <t>8701ER</t>
-  </si>
-  <si>
-    <t>2948II</t>
-  </si>
-  <si>
-    <t>2030PP</t>
-  </si>
-  <si>
-    <t>8239TT</t>
-  </si>
-  <si>
-    <t>Enschede</t>
-  </si>
-  <si>
-    <t>Denekamp</t>
-  </si>
-  <si>
-    <t>Ootmarsum</t>
-  </si>
-  <si>
-    <t>Oldenzaal</t>
-  </si>
-  <si>
-    <t>Neede</t>
-  </si>
-  <si>
-    <t>Losser</t>
-  </si>
-  <si>
-    <t>Hengelo</t>
-  </si>
-  <si>
-    <t>Almelo</t>
-  </si>
-  <si>
-    <t>WAG</t>
-  </si>
-  <si>
-    <t>RSK</t>
-  </si>
-  <si>
-    <t>MNS</t>
-  </si>
-  <si>
-    <t>HMN</t>
-  </si>
-  <si>
-    <t>KAD</t>
-  </si>
-  <si>
-    <t>BOT</t>
-  </si>
-  <si>
-    <t>ROG</t>
-  </si>
-  <si>
-    <t>VIK</t>
-  </si>
-  <si>
-    <t>HEE</t>
-  </si>
-  <si>
-    <t>KRO</t>
-  </si>
-  <si>
-    <t>gerard</t>
-  </si>
-  <si>
-    <t>marcel</t>
-  </si>
-  <si>
-    <t>pieter</t>
-  </si>
-  <si>
-    <t>cees</t>
-  </si>
-  <si>
-    <t>aad</t>
-  </si>
-  <si>
-    <t>karel</t>
-  </si>
-  <si>
-    <t>angela</t>
-  </si>
-  <si>
-    <t>merel</t>
-  </si>
-  <si>
-    <t>arnold</t>
-  </si>
-  <si>
-    <t>vincent</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,31 +748,31 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="7">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -780,31 +780,31 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -812,267 +812,267 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="7">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7">
         <v>24</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="7">
         <v>87</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="7">
         <v>23</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="7">
         <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="7">
         <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="7">
         <v>4</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="7">
         <v>5</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>